<commit_message>
Improving report and adding new tests output
</commit_message>
<xml_diff>
--- a/src/test/resources/report.xlsx
+++ b/src/test/resources/report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\140688330213\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\qsplitter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Number of Ids</t>
   </si>
@@ -40,6 +40,12 @@
   <si>
     <t>Temp Table of Ids</t>
   </si>
+  <si>
+    <t>Union All</t>
+  </si>
+  <si>
+    <t>Multi-Values In</t>
+  </si>
 </sst>
 </file>
 
@@ -54,12 +60,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="12"/>
+      <color rgb="FFD8D8D8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,7 +88,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -780,6 +786,310 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Union All</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$G$2:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1069</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1755</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1566</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1574</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1777</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Multi-Values In</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$H$2:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1027</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1878</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2211</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2397</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2709</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2843</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -789,11 +1099,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-748351360"/>
-        <c:axId val="-748338848"/>
+        <c:axId val="1316660336"/>
+        <c:axId val="1316657072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-748351360"/>
+        <c:axId val="1316660336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,7 +1193,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-748338848"/>
+        <c:crossAx val="1316657072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -891,7 +1201,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-748338848"/>
+        <c:axId val="1316657072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -990,7 +1300,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-748351360"/>
+        <c:crossAx val="1316660336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1598,6 +1908,310 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Union All</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$G$2:$G$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>735</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>756</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>788</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>839</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>881</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1069</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1385</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1755</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1566</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1574</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1777</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1932</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2188</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Multi-Values In</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Plan1!$H$2:$H$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>848</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>789</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>784</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>914</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1027</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1341</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1878</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2397</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2211</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2397</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2709</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2843</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1607,11 +2221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-748338304"/>
-        <c:axId val="-748357888"/>
+        <c:axId val="1316666320"/>
+        <c:axId val="1316653264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-748338304"/>
+        <c:axId val="1316666320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +2315,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-748357888"/>
+        <c:crossAx val="1316653264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1709,10 +2323,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-748357888"/>
+        <c:axId val="1316653264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3200"/>
+          <c:max val="3000"/>
+          <c:min val="600"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1808,7 +2423,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-748338304"/>
+        <c:crossAx val="1316666320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -3006,16 +3621,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3334,8 +3949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3345,6 +3960,8 @@
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3363,8 +3980,14 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -3380,8 +4003,17 @@
       <c r="F2">
         <v>661</v>
       </c>
+      <c r="G2">
+        <v>717</v>
+      </c>
+      <c r="H2">
+        <v>848</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2000</v>
       </c>
@@ -3397,8 +4029,17 @@
       <c r="F3">
         <v>671</v>
       </c>
+      <c r="G3">
+        <v>735</v>
+      </c>
+      <c r="H3">
+        <v>796</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3000</v>
       </c>
@@ -3414,8 +4055,17 @@
       <c r="F4">
         <v>684</v>
       </c>
+      <c r="G4">
+        <v>756</v>
+      </c>
+      <c r="H4">
+        <v>789</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4000</v>
       </c>
@@ -3431,8 +4081,17 @@
       <c r="F5">
         <v>701</v>
       </c>
+      <c r="G5">
+        <v>788</v>
+      </c>
+      <c r="H5">
+        <v>801</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5000</v>
       </c>
@@ -3448,8 +4107,17 @@
       <c r="F6">
         <v>713</v>
       </c>
+      <c r="G6">
+        <v>733</v>
+      </c>
+      <c r="H6">
+        <v>784</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6000</v>
       </c>
@@ -3465,8 +4133,17 @@
       <c r="F7">
         <v>731</v>
       </c>
+      <c r="G7">
+        <v>773</v>
+      </c>
+      <c r="H7">
+        <v>857</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7000</v>
       </c>
@@ -3482,8 +4159,17 @@
       <c r="F8">
         <v>746</v>
       </c>
+      <c r="G8">
+        <v>839</v>
+      </c>
+      <c r="H8">
+        <v>914</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8000</v>
       </c>
@@ -3499,8 +4185,17 @@
       <c r="F9">
         <v>779</v>
       </c>
+      <c r="G9">
+        <v>824</v>
+      </c>
+      <c r="H9">
+        <v>1148</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -3516,8 +4211,17 @@
       <c r="F10">
         <v>803</v>
       </c>
+      <c r="G10">
+        <v>844</v>
+      </c>
+      <c r="H10">
+        <v>1099</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10000</v>
       </c>
@@ -3533,9 +4237,17 @@
       <c r="F11">
         <v>818</v>
       </c>
+      <c r="G11">
+        <v>881</v>
+      </c>
+      <c r="H11">
+        <v>1027</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20000</v>
       </c>
@@ -3551,8 +4263,17 @@
       <c r="F12">
         <v>946</v>
       </c>
+      <c r="G12">
+        <v>1069</v>
+      </c>
+      <c r="H12">
+        <v>1463</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>30000</v>
       </c>
@@ -3568,8 +4289,17 @@
       <c r="F13">
         <v>1064</v>
       </c>
+      <c r="G13">
+        <v>1385</v>
+      </c>
+      <c r="H13">
+        <v>1341</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40000</v>
       </c>
@@ -3585,8 +4315,17 @@
       <c r="F14">
         <v>1184</v>
       </c>
+      <c r="G14">
+        <v>1755</v>
+      </c>
+      <c r="H14">
+        <v>1878</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50000</v>
       </c>
@@ -3602,8 +4341,17 @@
       <c r="F15">
         <v>1319</v>
       </c>
+      <c r="G15">
+        <v>1566</v>
+      </c>
+      <c r="H15">
+        <v>1995</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>60000</v>
       </c>
@@ -3619,8 +4367,17 @@
       <c r="F16">
         <v>1453</v>
       </c>
+      <c r="G16">
+        <v>1574</v>
+      </c>
+      <c r="H16">
+        <v>2397</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70000</v>
       </c>
@@ -3636,8 +4393,17 @@
       <c r="F17">
         <v>1574</v>
       </c>
+      <c r="G17">
+        <v>1777</v>
+      </c>
+      <c r="H17">
+        <v>2211</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80000</v>
       </c>
@@ -3653,8 +4419,17 @@
       <c r="F18">
         <v>1728</v>
       </c>
+      <c r="G18">
+        <v>2045</v>
+      </c>
+      <c r="H18">
+        <v>2397</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>90000</v>
       </c>
@@ -3670,8 +4445,17 @@
       <c r="F19">
         <v>1845</v>
       </c>
+      <c r="G19">
+        <v>1932</v>
+      </c>
+      <c r="H19">
+        <v>2709</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>100000</v>
       </c>
@@ -3687,6 +4471,15 @@
       <c r="F20">
         <v>2112</v>
       </c>
+      <c r="G20">
+        <v>2188</v>
+      </c>
+      <c r="H20">
+        <v>2843</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Renaming methods, fixing typos e improving some code snippet
</commit_message>
<xml_diff>
--- a/src/test/resources/report.xlsx
+++ b/src/test/resources/report.xlsx
@@ -182,7 +182,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Isolated In Clauses</c:v>
+            <c:v>N Queries</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -334,7 +334,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Disjunctions of In Clauses</c:v>
+            <c:v>Disjunctions of Expression Lists</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -483,162 +483,10 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Disjunctions of Ids</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Plan1!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>70000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>100000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Plan1!$E$2:$E$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>755</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>721</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>698</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>762</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>736</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>777</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>775</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>802</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>867</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>924</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1040</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1418</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1438</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1711</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1894</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2078</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2162</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2305</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2608</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Temp Table of Ids</c:v>
+            <c:v>Temp Table</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -788,7 +636,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Union All</c:v>
           </c:tx>
@@ -940,9 +788,9 @@
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:order val="4"/>
           <c:tx>
-            <c:v>Multi-Values In</c:v>
+            <c:v>Multivalued Expression Lists</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1099,11 +947,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1316660336"/>
-        <c:axId val="1316657072"/>
+        <c:axId val="-598001904"/>
+        <c:axId val="-598000816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1316660336"/>
+        <c:axId val="-598001904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1193,7 +1041,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316657072"/>
+        <c:crossAx val="-598000816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1201,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1316657072"/>
+        <c:axId val="-598000816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10000"/>
@@ -1300,7 +1148,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316660336"/>
+        <c:crossAx val="-598001904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1456,7 +1304,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Disjunctions of In Clauses</c:v>
+            <c:v>Disjunctions of Expression Lists</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1605,162 +1453,10 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Disjunctions of Ids</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Plan1!$A$2:$A$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>1000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>70000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>100000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Plan1!$E$2:$E$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
-                <c:pt idx="0">
-                  <c:v>755</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>721</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>698</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>762</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>736</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>777</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>775</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>802</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>867</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>924</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1040</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1418</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1438</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1711</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1894</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2078</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2162</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2305</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2608</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Temp Table of Ids</c:v>
+            <c:v>Temp Table</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1910,7 +1606,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Union All</c:v>
           </c:tx>
@@ -2062,9 +1758,9 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Multi-Values In</c:v>
+            <c:v>Multivalued Expression Lists</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -2221,11 +1917,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1316666320"/>
-        <c:axId val="1316653264"/>
+        <c:axId val="-388127456"/>
+        <c:axId val="-388125824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1316666320"/>
+        <c:axId val="-388127456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,7 +2011,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316653264"/>
+        <c:crossAx val="-388125824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2323,7 +2019,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1316653264"/>
+        <c:axId val="-388125824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000"/>
@@ -2423,7 +2119,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1316666320"/>
+        <c:crossAx val="-388127456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="200"/>
@@ -3949,8 +3645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>